<commit_message>
working on mongoDB and saveing pnr,booking id or if user cancel ticket then save status
</commit_message>
<xml_diff>
--- a/TBO_PNR_INFO_FOR_BOTH_LCC_OR_NO_LCC.xlsx
+++ b/TBO_PNR_INFO_FOR_BOTH_LCC_OR_NO_LCC.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>PNR</t>
   </si>
@@ -81,13 +81,69 @@
   </si>
   <si>
     <t> 1732238</t>
+  </si>
+  <si>
+    <t>'QG2I2Z'</t>
+  </si>
+  <si>
+    <t>YF8RSS</t>
+  </si>
+  <si>
+    <t>ticket id</t>
+  </si>
+  <si>
+    <r>
+      <t>"PNR"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"UYM6SB"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <t>BookingId: 1732697,</t>
+  </si>
+  <si>
+    <t>PNR: 'HMEYJH',</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    BookingId: 1732700</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PNR: 'XIC39G',</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      BookingId: 1732703,</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,6 +193,18 @@
       <color rgb="FF202020"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFA31515"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -159,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -172,9 +240,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -182,6 +247,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -463,32 +537,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.140625" style="8"/>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
@@ -500,34 +575,37 @@
       <c r="E2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="8">
         <v>1732238</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <v>1732373</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <v>1732384</v>
       </c>
       <c r="C5" t="s">
@@ -540,11 +618,11 @@
         <v>285854</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <v>1732389</v>
       </c>
       <c r="C6" t="s">
@@ -554,11 +632,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="7">
         <v>1732595</v>
       </c>
       <c r="C7" t="s">
@@ -571,11 +649,11 @@
         <v>285853</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="7">
         <v>1732602</v>
       </c>
       <c r="C8" t="s">
@@ -585,20 +663,63 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="8">
         <v>1732082</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="7">
+        <v>1732693</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="4">
+        <v>1732696</v>
+      </c>
+      <c r="F12" s="4">
+        <v>2012091</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>